<commit_message>
added scrapped data from monsters, now with duplicates removal and proper records
</commit_message>
<xml_diff>
--- a/database/w3/Ninjutsu_Scroll.xlsx
+++ b/database/w3/Ninjutsu_Scroll.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Water Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Critical Rate5</t>
+          <t>Ailment Resistance %
+5
+Magic Device only:Aggro %-10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,12 +488,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Earth Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Critical Rate5</t>
+          <t>MaxHP %
+101
+-Handed Sword only:Fractional Barrier %10</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -509,12 +513,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Wind Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Critical Rate5</t>
+          <t>ASPD
+250
+Katana only:Critical Rate5</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -532,66 +538,64 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Critical Rate5</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>empty</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sell1 SpinaProcess2 Wood</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Lightning Ninjutsu Scroll[Ninjutsu Scroll]</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Stability %
+5
+Katana only:Accuracy %10</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>empty</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sell1 SpinaProcess2 Wood</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Fire Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>MATK %
 1
 Staff only:Magic Pierce %5</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Lightning Ninjutsu Scroll[Ninjutsu Scroll]</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Stability %
-5
-Katana only:Accuracy %10</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Water Ninjutsu Scroll[Ninjutsu Scroll]</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Ailment Resistance %
-5
-Magic Device only:Aggro %-10</t>
-        </is>
-      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>empty</t>
@@ -607,14 +611,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Earth Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Dark Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MaxHP %
-101
--Handed Sword only:Fractional Barrier %10</t>
+          <t>Aggro %-10</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -628,54 +630,6 @@
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Wind Ninjutsu Scroll[Ninjutsu Scroll]</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ASPD
-250
-Katana only:Critical Rate5</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Dark Ninjutsu Scroll[Ninjutsu Scroll]</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Aggro %-10</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adding an upgrade to overall system with extra renderer
</commit_message>
<xml_diff>
--- a/database/w3/Ninjutsu_Scroll.xlsx
+++ b/database/w3/Ninjutsu_Scroll.xlsx
@@ -463,14 +463,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Water Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Lightning Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ailment Resistance %
-5
-Magic Device only:Aggro %-10</t>
+          <t>Stability %
+5Katana only:Accuracy %
+10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -488,14 +488,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fire Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Water Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MATK %
-1
-Staff only:Magic Pierce %5</t>
+          <t>Ailment Resistance %
+5Magic Device only:
+Aggro %
+-10</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -518,9 +519,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MaxHP %
-101
--Handed Sword only:Fractional Barrier %10</t>
+          <t xml:space="preserve">
+MaxHP %
+101-Handed Sword only:Fractional 
+Barrier %
+10</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -538,14 +541,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Wind Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ASPD
-250
-Katana only:Critical Rate5</t>
+          <t xml:space="preserve">
+Critical Rate
+5</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -563,14 +566,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lightning Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Fire Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Stability %
-5
-Katana only:Accuracy %10</t>
+          <t>MATK
+ %
+1Staff only:Magic Pierce %
+5</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -588,12 +592,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dark Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Wind Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Aggro %-10</t>
+          <t xml:space="preserve">
+ASPD250Katana only:
+Critical Rate
+5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -611,12 +618,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Dark Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Critical Rate5</t>
+          <t xml:space="preserve">
+Aggro %
+-10</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>

<commit_message>
if it works it works, now works with docker bich
</commit_message>
<xml_diff>
--- a/database/w3/Ninjutsu_Scroll.xlsx
+++ b/database/w3/Ninjutsu_Scroll.xlsx
@@ -463,14 +463,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lightning Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Fire Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Stability %
-5Katana only:Accuracy %
-10</t>
+          <t>MATK
+ %
+1Staff only:Magic Pierce %
+5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,7 +481,10 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
+          <t>Sell1
+Spina
+Process
+2 Wood</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -488,10 +492,127 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Wind Ninjutsu Scroll[Ninjutsu Scroll]</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ASPD250Katana only:
+Critical Rate
+5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>empty</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Sell1
+Spina
+Process
+2 Wood</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Lightning Ninjutsu Scroll[Ninjutsu Scroll]</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Stability %
+5Katana only:
+Accuracy %
+10</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>empty</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Sell1
+Spina
+Process
+2 Wood</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Critical Rate
+5</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>empty</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sell1
+Spina
+Process
+2 Wood</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Earth Ninjutsu Scroll[Ninjutsu Scroll]</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+MaxHP
+ %
+101-Handed Sword only:Fractional 
+Barrier %
+10</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>empty</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sell1
+Spina
+Process
+2 Wood</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Water Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>Ailment Resistance %
 5Magic Device only:
@@ -499,118 +620,17 @@
 -10</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>empty</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Earth Ninjutsu Scroll[Ninjutsu Scroll]</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-MaxHP %
-101-Handed Sword only:Fractional 
-Barrier %
-10</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Critical Rate
-5</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Fire Ninjutsu Scroll[Ninjutsu Scroll]</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>MATK
- %
-1Staff only:Magic Pierce %
-5</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Wind Ninjutsu Scroll[Ninjutsu Scroll]</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-ASPD250Katana only:
-Critical Rate
-5</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
+          <t>Sell1
+Spina
+Process
+2 Wood</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -635,7 +655,10 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sell1 SpinaProcess2 Wood</t>
+          <t>Sell1
+Spina
+Process
+2 Wood</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>

</xml_diff>

<commit_message>
new front end page with better display database
</commit_message>
<xml_diff>
--- a/database/w3/Ninjutsu_Scroll.xlsx
+++ b/database/w3/Ninjutsu_Scroll.xlsx
@@ -463,15 +463,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fire Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Dark Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MATK
- %
-1Staff only:Magic Pierce %
-5</t>
+          <t>Aggro %
+- 10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -492,15 +490,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wind Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Water Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-ASPD250Katana only:
-Critical Rate
-5</t>
+          <t>Ailment Resistance %
+5
+Magic Device only:Aggro %
+- 10</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -521,15 +519,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lightning Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Stability %
-5Katana only:
-Accuracy %
-10</t>
+          <t>Critical Rate
+5</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -550,13 +546,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Metal Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Wind Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Critical Rate
+          <t>ASPD
+250
+Katana only:Critical Rate
 5</t>
         </is>
       </c>
@@ -583,11 +580,9 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-MaxHP
- %
-101-Handed Sword only:Fractional 
-Barrier %
+          <t>Max HP %
+101
+-Handed Sword only:Fractional Barrier %
 10</t>
         </is>
       </c>
@@ -609,15 +604,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Water Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Fire Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ailment Resistance %
-5Magic Device only:
-Aggro %
--10</t>
+          <t>MATK %
+1
+Staff only:Magic Pierce %
+5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -638,14 +633,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Dark Ninjutsu Scroll[Ninjutsu Scroll]</t>
+          <t>Lightning Ninjutsu Scroll[Ninjutsu Scroll]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Aggro %
--10</t>
+          <t>Stability %
+5
+Katana only:Accuracy %
+10</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>